<commit_message>
add one printer check
</commit_message>
<xml_diff>
--- a/ip_addresses.xlsx
+++ b/ip_addresses.xlsx
@@ -16,7 +16,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="116">
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>10.160.13.201</t>
+  </si>
+  <si>
+    <t>10.160.13.202</t>
+  </si>
+  <si>
+    <t>10.160.13.203</t>
+  </si>
+  <si>
+    <t>10.160.13.204</t>
+  </si>
+  <si>
+    <t>10.160.13.205</t>
+  </si>
+  <si>
+    <t>10.160.13.206</t>
+  </si>
+  <si>
+    <t>10.160.13.207</t>
+  </si>
+  <si>
+    <t>10.160.13.208</t>
+  </si>
+  <si>
+    <t>10.160.13.210</t>
+  </si>
+  <si>
+    <t>10.160.13.211</t>
+  </si>
   <si>
     <t>10.160.167.202</t>
   </si>
@@ -42,23 +81,296 @@
     <t>10.160.167.209</t>
   </si>
   <si>
-    <t>public</t>
-  </si>
-  <si>
-    <t>IP Address</t>
-  </si>
-  <si>
-    <t>Community</t>
-  </si>
-  <si>
-    <t>10.160.167.999</t>
+    <t>10.160.179.147</t>
+  </si>
+  <si>
+    <t>10.160.179.148</t>
+  </si>
+  <si>
+    <t>10.160.179.149</t>
+  </si>
+  <si>
+    <t>10.160.183.201</t>
+  </si>
+  <si>
+    <t>10.160.183.202</t>
+  </si>
+  <si>
+    <t>10.160.38.204</t>
+  </si>
+  <si>
+    <t>10.160.38.207</t>
+  </si>
+  <si>
+    <t>10.160.38.209</t>
+  </si>
+  <si>
+    <t>10.160.38.210</t>
+  </si>
+  <si>
+    <t>10.160.38.211</t>
+  </si>
+  <si>
+    <t>10.160.38.212</t>
+  </si>
+  <si>
+    <t>10.160.38.213</t>
+  </si>
+  <si>
+    <t>10.160.38.214</t>
+  </si>
+  <si>
+    <t>10.160.43.203</t>
+  </si>
+  <si>
+    <t>10.160.43.204</t>
+  </si>
+  <si>
+    <t>10.160.43.205</t>
+  </si>
+  <si>
+    <t>10.160.43.206</t>
+  </si>
+  <si>
+    <t>10.160.43.207</t>
+  </si>
+  <si>
+    <t>10.160.43.208</t>
+  </si>
+  <si>
+    <t>10.160.43.209</t>
+  </si>
+  <si>
+    <t>10.160.184.199</t>
+  </si>
+  <si>
+    <t>10.160.184.200</t>
+  </si>
+  <si>
+    <t>10.160.57.202</t>
+  </si>
+  <si>
+    <t>10.160.57.203</t>
+  </si>
+  <si>
+    <t>10.160.57.204</t>
+  </si>
+  <si>
+    <t>10.160.57.205</t>
+  </si>
+  <si>
+    <t>10.160.57.208</t>
+  </si>
+  <si>
+    <t>10.160.57.209</t>
+  </si>
+  <si>
+    <t>10.160.57.210</t>
+  </si>
+  <si>
+    <t>10.160.57.211</t>
+  </si>
+  <si>
+    <t>10.160.57.212</t>
+  </si>
+  <si>
+    <t>10.160.57.213</t>
+  </si>
+  <si>
+    <t>10.160.57.214</t>
+  </si>
+  <si>
+    <t>10.160.66.201</t>
+  </si>
+  <si>
+    <t>10.160.66.202</t>
+  </si>
+  <si>
+    <t>10.160.66.203</t>
+  </si>
+  <si>
+    <t>10.160.66.204</t>
+  </si>
+  <si>
+    <t>10.160.66.205</t>
+  </si>
+  <si>
+    <t>10.160.66.206</t>
+  </si>
+  <si>
+    <t>10.160.66.208</t>
+  </si>
+  <si>
+    <t>10.160.66.211</t>
+  </si>
+  <si>
+    <t>10.160.66.212</t>
+  </si>
+  <si>
+    <t>10.160.66.213</t>
+  </si>
+  <si>
+    <t>10.20.0.104</t>
+  </si>
+  <si>
+    <t>10.160.179.109</t>
+  </si>
+  <si>
+    <t>10.160.179.146</t>
+  </si>
+  <si>
+    <t>10.160.179.139</t>
+  </si>
+  <si>
+    <t>10.20.0.115</t>
+  </si>
+  <si>
+    <t>10.20.0.150</t>
+  </si>
+  <si>
+    <t>10.160.179.111</t>
+  </si>
+  <si>
+    <t>10.160.179.134</t>
+  </si>
+  <si>
+    <t>10.160.179.110</t>
+  </si>
+  <si>
+    <t>10.160.179.120</t>
+  </si>
+  <si>
+    <t>10.160.179.135</t>
+  </si>
+  <si>
+    <t>10.160.179.141</t>
+  </si>
+  <si>
+    <t>10.160.179.130</t>
+  </si>
+  <si>
+    <t>10.160.179.133</t>
+  </si>
+  <si>
+    <t>10.160.179.123</t>
+  </si>
+  <si>
+    <t>10.160.179.128</t>
+  </si>
+  <si>
+    <t>10.160.179.119</t>
+  </si>
+  <si>
+    <t>10.20.0.227</t>
+  </si>
+  <si>
+    <t>10.160.179.127</t>
+  </si>
+  <si>
+    <t>10.160.179.112</t>
+  </si>
+  <si>
+    <t>10.160.179.143</t>
+  </si>
+  <si>
+    <t>10.20.0.234</t>
+  </si>
+  <si>
+    <t>10.160.179.113</t>
+  </si>
+  <si>
+    <t>10.160.179.108</t>
+  </si>
+  <si>
+    <t>10.160.179.144</t>
+  </si>
+  <si>
+    <t>10.20.0.83</t>
+  </si>
+  <si>
+    <t>10.160.179.142</t>
+  </si>
+  <si>
+    <t>10.160.179.118</t>
+  </si>
+  <si>
+    <t>10.160.179.103</t>
+  </si>
+  <si>
+    <t>10.160.179.104</t>
+  </si>
+  <si>
+    <t>10.160.179.136</t>
+  </si>
+  <si>
+    <t>10.160.179.105</t>
+  </si>
+  <si>
+    <t>10.160.179.106</t>
+  </si>
+  <si>
+    <t>10.160.179.107</t>
+  </si>
+  <si>
+    <t>10.160.179.132</t>
+  </si>
+  <si>
+    <t>10.160.179.145</t>
+  </si>
+  <si>
+    <t>10.160.179.116</t>
+  </si>
+  <si>
+    <t>10.160.179.126</t>
+  </si>
+  <si>
+    <t>10.160.179.125</t>
+  </si>
+  <si>
+    <t>10.160.179.121</t>
+  </si>
+  <si>
+    <t>10.160.179.124</t>
+  </si>
+  <si>
+    <t>10.160.179.115</t>
+  </si>
+  <si>
+    <t>10.160.52.203</t>
+  </si>
+  <si>
+    <t>10.160.52.204</t>
+  </si>
+  <si>
+    <t>10.160.52.205</t>
+  </si>
+  <si>
+    <t>10.160.52.206</t>
+  </si>
+  <si>
+    <t>10.160.52.207</t>
+  </si>
+  <si>
+    <t>10.160.52.208</t>
+  </si>
+  <si>
+    <t>10.160.52.209</t>
+  </si>
+  <si>
+    <t>10.160.52.211</t>
+  </si>
+  <si>
+    <t>10.160.52.201</t>
+  </si>
+  <si>
+    <t>10.160.52.202</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,8 +634,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,8 +863,20 @@
         <bgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -676,8 +1006,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="70">
+  <cellStyleXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -751,11 +1096,99 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="70">
+  <cellStyles count="148">
     <cellStyle name="20% - 1. jelölőszín" xfId="18" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - 2. jelölőszín" xfId="22" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - 3. jelölőszín" xfId="26" builtinId="38" customBuiltin="1"/>
@@ -796,6 +1229,7 @@
     <cellStyle name="Hivatkozás 2" xfId="52"/>
     <cellStyle name="Hivatkozás 3" xfId="53"/>
     <cellStyle name="Hivatkozott cella" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Jegyzet" xfId="70" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Jegyzet 2" xfId="54"/>
     <cellStyle name="Jelölőszín (1)" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Jelölőszín (2)" xfId="21" builtinId="33" customBuiltin="1"/>
@@ -808,14 +1242,91 @@
     <cellStyle name="Magyarázó szöveg" xfId="15" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="55"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál 2" xfId="101"/>
+    <cellStyle name="Normál 2 10" xfId="132"/>
+    <cellStyle name="Normál 2 11" xfId="138"/>
+    <cellStyle name="Normál 2 12" xfId="131"/>
+    <cellStyle name="Normál 2 13" xfId="139"/>
+    <cellStyle name="Normál 2 14" xfId="129"/>
+    <cellStyle name="Normál 2 15" xfId="140"/>
     <cellStyle name="Normál 2 2" xfId="56"/>
+    <cellStyle name="Normál 2 2 10" xfId="98"/>
+    <cellStyle name="Normál 2 2 11" xfId="95"/>
+    <cellStyle name="Normál 2 2 12" xfId="74"/>
+    <cellStyle name="Normál 2 2 13" xfId="111"/>
+    <cellStyle name="Normál 2 2 14" xfId="87"/>
+    <cellStyle name="Normál 2 2 15" xfId="115"/>
+    <cellStyle name="Normál 2 2 16" xfId="116"/>
+    <cellStyle name="Normál 2 2 17" xfId="118"/>
+    <cellStyle name="Normál 2 2 18" xfId="119"/>
+    <cellStyle name="Normál 2 2 19" xfId="120"/>
     <cellStyle name="Normál 2 2 2" xfId="57"/>
+    <cellStyle name="Normál 2 2 2 10" xfId="80"/>
+    <cellStyle name="Normál 2 2 2 11" xfId="117"/>
+    <cellStyle name="Normál 2 2 2 12" xfId="97"/>
+    <cellStyle name="Normál 2 2 2 13" xfId="82"/>
+    <cellStyle name="Normál 2 2 2 14" xfId="77"/>
+    <cellStyle name="Normál 2 2 2 15" xfId="81"/>
+    <cellStyle name="Normál 2 2 2 16" xfId="96"/>
+    <cellStyle name="Normál 2 2 2 17" xfId="73"/>
+    <cellStyle name="Normál 2 2 2 18" xfId="75"/>
+    <cellStyle name="Normál 2 2 2 19" xfId="121"/>
     <cellStyle name="Normál 2 2 2 2" xfId="58"/>
+    <cellStyle name="Normál 2 2 2 20" xfId="124"/>
+    <cellStyle name="Normál 2 2 2 3" xfId="110"/>
+    <cellStyle name="Normál 2 2 2 4" xfId="91"/>
+    <cellStyle name="Normál 2 2 2 5" xfId="106"/>
+    <cellStyle name="Normál 2 2 2 6" xfId="88"/>
+    <cellStyle name="Normál 2 2 2 7" xfId="108"/>
+    <cellStyle name="Normál 2 2 2 8" xfId="84"/>
+    <cellStyle name="Normál 2 2 2 9" xfId="86"/>
+    <cellStyle name="Normál 2 2 20" xfId="123"/>
+    <cellStyle name="Normál 2 2 3" xfId="109"/>
+    <cellStyle name="Normál 2 2 4" xfId="93"/>
+    <cellStyle name="Normál 2 2 5" xfId="104"/>
+    <cellStyle name="Normál 2 2 6" xfId="71"/>
+    <cellStyle name="Normál 2 2 7" xfId="72"/>
+    <cellStyle name="Normál 2 2 8" xfId="78"/>
+    <cellStyle name="Normál 2 2 9" xfId="113"/>
     <cellStyle name="Normál 2 3" xfId="59"/>
     <cellStyle name="Normál 2 4" xfId="60"/>
+    <cellStyle name="Normál 2 5" xfId="136"/>
+    <cellStyle name="Normál 2 6" xfId="134"/>
+    <cellStyle name="Normál 2 7" xfId="137"/>
+    <cellStyle name="Normál 2 8" xfId="133"/>
+    <cellStyle name="Normál 2 9" xfId="135"/>
     <cellStyle name="Normál 3" xfId="61"/>
+    <cellStyle name="Normál 3 10" xfId="92"/>
+    <cellStyle name="Normál 3 10 2" xfId="144"/>
+    <cellStyle name="Normál 3 11" xfId="105"/>
+    <cellStyle name="Normál 3 11 2" xfId="126"/>
+    <cellStyle name="Normál 3 12" xfId="94"/>
+    <cellStyle name="Normál 3 12 2" xfId="145"/>
+    <cellStyle name="Normál 3 13" xfId="79"/>
+    <cellStyle name="Normál 3 13 2" xfId="147"/>
+    <cellStyle name="Normál 3 14" xfId="100"/>
+    <cellStyle name="Normál 3 14 2" xfId="146"/>
+    <cellStyle name="Normál 3 15" xfId="103"/>
+    <cellStyle name="Normál 3 16" xfId="102"/>
+    <cellStyle name="Normál 3 17" xfId="76"/>
+    <cellStyle name="Normál 3 18" xfId="114"/>
+    <cellStyle name="Normál 3 19" xfId="90"/>
     <cellStyle name="Normál 3 2" xfId="62"/>
+    <cellStyle name="Normál 3 20" xfId="122"/>
+    <cellStyle name="Normál 3 21" xfId="125"/>
     <cellStyle name="Normál 3 3" xfId="63"/>
+    <cellStyle name="Normál 3 4" xfId="112"/>
+    <cellStyle name="Normál 3 4 2" xfId="141"/>
+    <cellStyle name="Normál 3 5" xfId="85"/>
+    <cellStyle name="Normál 3 5 2" xfId="130"/>
+    <cellStyle name="Normál 3 6" xfId="83"/>
+    <cellStyle name="Normál 3 6 2" xfId="142"/>
+    <cellStyle name="Normál 3 7" xfId="89"/>
+    <cellStyle name="Normál 3 7 2" xfId="128"/>
+    <cellStyle name="Normál 3 8" xfId="107"/>
+    <cellStyle name="Normál 3 8 2" xfId="143"/>
+    <cellStyle name="Normál 3 9" xfId="99"/>
+    <cellStyle name="Normál 3 9 2" xfId="127"/>
     <cellStyle name="Normál 4" xfId="64"/>
     <cellStyle name="Normál 5" xfId="65"/>
     <cellStyle name="Note" xfId="66"/>
@@ -1117,96 +1628,928 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B62" sqref="B61:B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>